<commit_message>
amend USB Type A connector Power Supply
</commit_message>
<xml_diff>
--- a/BOM_LIST.xlsx
+++ b/BOM_LIST.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\app01\APIC\SAM\20200427_SAMD21G_TrainingBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5C19D9-1C31-48B6-AC0E-E25A5AEA6E52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0230EC-1694-4924-8591-F0C9EE61BC7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9615" yWindow="555" windowWidth="15975" windowHeight="14895" xr2:uid="{6FC32BAF-5541-4079-8905-E17F7838DA01}"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="24150" windowHeight="15990" xr2:uid="{6FC32BAF-5541-4079-8905-E17F7838DA01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet3!$A$5:$L$79</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="226">
   <si>
     <t>ref</t>
   </si>
@@ -971,6 +974,20 @@
     <rPh sb="0" eb="1">
       <t>エン</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>※下記ピンヘッダ切断</t>
+    <rPh sb="1" eb="3">
+      <t>カキ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>セツダン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>〃</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -978,7 +995,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1010,6 +1027,15 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1020,83 +1046,23 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
+        <fgColor theme="1" tint="0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1109,11 +1075,135 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1125,56 +1215,71 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1667,9 +1772,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC5E10D-FBC2-4E44-A005-8F442C956AC0}">
-  <dimension ref="A1:K79"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K50" sqref="K50"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -1681,2244 +1791,2255 @@
     <col min="6" max="6" width="19.25" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.25" style="1" customWidth="1"/>
     <col min="8" max="10" width="9" style="1"/>
-    <col min="11" max="11" width="13.25" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19.625" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A5" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="C5" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="13" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="H6" s="7">
-        <v>1</v>
-      </c>
-      <c r="I6" s="8">
+      <c r="H6" s="5">
+        <v>1</v>
+      </c>
+      <c r="I6" s="6">
         <v>530</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="5">
         <f>H6*I6</f>
         <v>530</v>
       </c>
-      <c r="K6" s="9"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A7" s="6" t="s">
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A7" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="H7" s="7">
-        <v>1</v>
-      </c>
-      <c r="I7" s="7">
+      <c r="H7" s="5">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5">
         <v>50</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="5">
         <f t="shared" ref="J7:J70" si="0">H7*I7</f>
         <v>50</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="K7" s="7" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A8" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="H8" s="7">
-        <v>1</v>
-      </c>
-      <c r="I8" s="7">
+      <c r="H8" s="5">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5">
         <v>155</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="5">
         <f t="shared" si="0"/>
         <v>155</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="K8" s="7" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A9" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="H9" s="7">
-        <v>1</v>
-      </c>
-      <c r="I9" s="7">
+      <c r="H9" s="5">
+        <v>1</v>
+      </c>
+      <c r="I9" s="5">
         <v>667</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="5">
         <f t="shared" si="0"/>
         <v>667</v>
       </c>
-      <c r="K9" s="9"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A10" s="6" t="s">
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A10" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="H10" s="7">
-        <v>1</v>
-      </c>
-      <c r="I10" s="7">
+      <c r="H10" s="5">
+        <v>1</v>
+      </c>
+      <c r="I10" s="5">
         <v>950</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="5">
         <f t="shared" si="0"/>
         <v>950</v>
       </c>
-      <c r="K10" s="9"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A11" s="6" t="s">
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A11" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="H11" s="7">
-        <v>1</v>
-      </c>
-      <c r="I11" s="7">
+      <c r="H11" s="5">
+        <v>1</v>
+      </c>
+      <c r="I11" s="5">
         <v>20</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="5">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="K11" s="9"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A12" s="6" t="s">
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A12" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="H12" s="7">
-        <v>1</v>
-      </c>
-      <c r="I12" s="7">
+      <c r="H12" s="5">
+        <v>1</v>
+      </c>
+      <c r="I12" s="5">
         <v>20</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="5">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="K12" s="9"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A13" s="6" t="s">
+      <c r="K12" s="7"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A13" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="H13" s="7">
-        <v>1</v>
-      </c>
-      <c r="I13" s="7">
+      <c r="H13" s="5">
+        <v>1</v>
+      </c>
+      <c r="I13" s="5">
         <v>20</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="5">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="K13" s="9"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A14" s="6" t="s">
+      <c r="K13" s="7"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A14" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="H14" s="7">
-        <v>1</v>
-      </c>
-      <c r="I14" s="7">
+      <c r="H14" s="5">
+        <v>1</v>
+      </c>
+      <c r="I14" s="5">
         <v>20</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="5">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="K14" s="9"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A15" s="6" t="s">
+      <c r="K14" s="7"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A15" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="H15" s="7">
-        <v>1</v>
-      </c>
-      <c r="I15" s="7">
+      <c r="H15" s="5">
+        <v>1</v>
+      </c>
+      <c r="I15" s="5">
         <v>140</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J15" s="5">
         <f t="shared" si="0"/>
         <v>140</v>
       </c>
-      <c r="K15" s="9"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A16" s="6" t="s">
+      <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A16" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="H16" s="7">
-        <v>1</v>
-      </c>
-      <c r="I16" s="7">
+      <c r="H16" s="5">
+        <v>1</v>
+      </c>
+      <c r="I16" s="5">
         <v>1080</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J16" s="5">
         <f t="shared" si="0"/>
         <v>1080</v>
       </c>
-      <c r="K16" s="9"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A17" s="6" t="s">
+      <c r="K16" s="7"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A17" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="H17" s="7">
-        <v>1</v>
-      </c>
-      <c r="I17" s="7">
+      <c r="H17" s="5">
+        <v>1</v>
+      </c>
+      <c r="I17" s="5">
         <v>10</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="K17" s="9"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A18" s="11" t="s">
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A18" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G18" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="H18" s="7">
-        <v>1</v>
-      </c>
-      <c r="I18" s="7">
+      <c r="H18" s="5">
+        <v>1</v>
+      </c>
+      <c r="I18" s="5">
         <v>10</v>
       </c>
-      <c r="J18" s="7">
+      <c r="J18" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="K18" s="9"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A19" s="6" t="s">
+      <c r="K18" s="7"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A19" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H19" s="7">
-        <v>1</v>
-      </c>
-      <c r="I19" s="7">
+      <c r="E19" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H19" s="5">
+        <v>1</v>
+      </c>
+      <c r="I19" s="5">
         <v>10</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J19" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="K19" s="9"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A20" s="6" t="s">
+      <c r="K19" s="7"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A20" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="H20" s="7">
-        <v>1</v>
-      </c>
-      <c r="I20" s="7">
+      <c r="H20" s="5">
+        <v>1</v>
+      </c>
+      <c r="I20" s="5">
         <v>20</v>
       </c>
-      <c r="J20" s="7">
+      <c r="J20" s="5">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="K20" s="9" t="s">
+      <c r="K20" s="7" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A21" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G21" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="H21" s="7">
-        <v>1</v>
-      </c>
-      <c r="I21" s="7">
+      <c r="H21" s="5">
+        <v>1</v>
+      </c>
+      <c r="I21" s="5">
         <v>20</v>
       </c>
-      <c r="J21" s="7">
+      <c r="J21" s="5">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="K21" s="9" t="s">
+      <c r="K21" s="7" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A22" s="6" t="s">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A22" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="H22" s="7">
-        <v>1</v>
-      </c>
-      <c r="I22" s="7">
+      <c r="H22" s="5">
+        <v>1</v>
+      </c>
+      <c r="I22" s="5">
         <v>50</v>
       </c>
-      <c r="J22" s="7">
+      <c r="J22" s="5">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="K22" s="9"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A23" s="6" t="s">
+      <c r="K22" s="7"/>
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A23" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H23" s="7">
-        <v>1</v>
-      </c>
-      <c r="I23" s="7">
+      <c r="E23" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H23" s="5">
+        <v>1</v>
+      </c>
+      <c r="I23" s="5">
         <v>50</v>
       </c>
-      <c r="J23" s="7">
+      <c r="J23" s="5">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="K23" s="9"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A24" s="6" t="s">
+      <c r="K23" s="7"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A24" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="G24" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="H24" s="8">
-        <v>1</v>
-      </c>
-      <c r="I24" s="8">
+      <c r="H24" s="6">
+        <v>1</v>
+      </c>
+      <c r="I24" s="6">
         <v>250</v>
       </c>
-      <c r="J24" s="7">
+      <c r="J24" s="5">
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
-      <c r="K24" s="9"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A25" s="6" t="s">
+      <c r="K24" s="7"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A25" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G25" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="H25" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="I25" s="8" t="s">
+      <c r="I25" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="J25" s="7"/>
-      <c r="K25" s="9" t="s">
+      <c r="J25" s="15"/>
+      <c r="K25" s="16" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A26" s="6" t="s">
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A26" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="G26" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="H26" s="7">
-        <v>1</v>
-      </c>
-      <c r="I26" s="7">
+      <c r="H26" s="5">
+        <v>1</v>
+      </c>
+      <c r="I26" s="5">
         <v>30</v>
       </c>
-      <c r="J26" s="7">
+      <c r="J26" s="5">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="K26" s="9"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A27" s="6" t="s">
+      <c r="K26" s="7"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A27" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="G27" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="H27" s="7">
-        <v>1</v>
-      </c>
-      <c r="I27" s="7">
+      <c r="H27" s="5">
+        <v>1</v>
+      </c>
+      <c r="I27" s="5">
         <v>10</v>
       </c>
-      <c r="J27" s="7">
+      <c r="J27" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="K27" s="9" t="s">
+      <c r="K27" s="7" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A28" s="6" t="s">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A28" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="G28" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="H28" s="7">
-        <v>1</v>
-      </c>
-      <c r="I28" s="7">
+      <c r="H28" s="5">
+        <v>1</v>
+      </c>
+      <c r="I28" s="5">
         <v>20</v>
       </c>
-      <c r="J28" s="7">
+      <c r="J28" s="5">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="K28" s="9" t="s">
+      <c r="K28" s="7" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A29" s="6" t="s">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A29" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H29" s="7">
-        <v>1</v>
-      </c>
-      <c r="I29" s="7">
+      <c r="E29" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H29" s="5">
+        <v>1</v>
+      </c>
+      <c r="I29" s="5">
         <v>20</v>
       </c>
-      <c r="J29" s="7">
+      <c r="J29" s="5">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="K29" s="9"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A30" s="6" t="s">
+      <c r="K29" s="7"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A30" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E30" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H30" s="7">
-        <v>1</v>
-      </c>
-      <c r="I30" s="7">
+      <c r="E30" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H30" s="5">
+        <v>1</v>
+      </c>
+      <c r="I30" s="5">
         <v>20</v>
       </c>
-      <c r="J30" s="7">
+      <c r="J30" s="5">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="K30" s="9"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A31" s="6" t="s">
+      <c r="K30" s="7"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A31" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H31" s="7">
-        <v>1</v>
-      </c>
-      <c r="I31" s="7">
+      <c r="E31" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H31" s="5">
+        <v>1</v>
+      </c>
+      <c r="I31" s="5">
         <v>20</v>
       </c>
-      <c r="J31" s="7">
+      <c r="J31" s="5">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="K31" s="9"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A32" s="6" t="s">
+      <c r="K31" s="7"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A32" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H32" s="7">
-        <v>1</v>
-      </c>
-      <c r="I32" s="7">
+      <c r="E32" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H32" s="5">
+        <v>1</v>
+      </c>
+      <c r="I32" s="5">
         <v>20</v>
       </c>
-      <c r="J32" s="7">
+      <c r="J32" s="5">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="K32" s="9"/>
+      <c r="K32" s="7"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E33" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H33" s="7">
-        <v>1</v>
-      </c>
-      <c r="I33" s="7">
+      <c r="E33" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H33" s="5">
+        <v>1</v>
+      </c>
+      <c r="I33" s="5">
         <v>20</v>
       </c>
-      <c r="J33" s="7">
+      <c r="J33" s="5">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="K33" s="9"/>
+      <c r="K33" s="7"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F34" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G34" s="7" t="s">
+      <c r="G34" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="H34" s="7">
-        <v>1</v>
-      </c>
-      <c r="I34" s="7">
+      <c r="H34" s="5">
+        <v>1</v>
+      </c>
+      <c r="I34" s="5">
         <v>10</v>
       </c>
-      <c r="J34" s="7">
+      <c r="J34" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="K34" s="9" t="s">
+      <c r="K34" s="7" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E35" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H35" s="7">
-        <v>1</v>
-      </c>
-      <c r="I35" s="7">
+      <c r="E35" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H35" s="5">
+        <v>1</v>
+      </c>
+      <c r="I35" s="5">
         <v>10</v>
       </c>
-      <c r="J35" s="7">
+      <c r="J35" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="K35" s="9"/>
+      <c r="K35" s="7"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E36" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H36" s="7">
-        <v>1</v>
-      </c>
-      <c r="I36" s="7">
+      <c r="E36" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H36" s="5">
+        <v>1</v>
+      </c>
+      <c r="I36" s="5">
         <v>10</v>
       </c>
-      <c r="J36" s="7">
+      <c r="J36" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="K36" s="9"/>
+      <c r="K36" s="7"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E37" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G37" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H37" s="7">
-        <v>1</v>
-      </c>
-      <c r="I37" s="7">
+      <c r="E37" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H37" s="5">
+        <v>1</v>
+      </c>
+      <c r="I37" s="5">
         <v>10</v>
       </c>
-      <c r="J37" s="7">
+      <c r="J37" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="K37" s="9"/>
+      <c r="K37" s="7"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E38" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H38" s="7">
-        <v>1</v>
-      </c>
-      <c r="I38" s="7">
+      <c r="E38" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H38" s="5">
+        <v>1</v>
+      </c>
+      <c r="I38" s="5">
         <v>10</v>
       </c>
-      <c r="J38" s="7">
+      <c r="J38" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="K38" s="9"/>
+      <c r="K38" s="7"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E39" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H39" s="7">
-        <v>1</v>
-      </c>
-      <c r="I39" s="7">
+      <c r="E39" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H39" s="5">
+        <v>1</v>
+      </c>
+      <c r="I39" s="5">
         <v>10</v>
       </c>
-      <c r="J39" s="7">
+      <c r="J39" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="K39" s="9"/>
+      <c r="K39" s="7"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E40" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H40" s="7">
-        <v>1</v>
-      </c>
-      <c r="I40" s="7">
+      <c r="E40" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H40" s="5">
+        <v>1</v>
+      </c>
+      <c r="I40" s="5">
         <v>10</v>
       </c>
-      <c r="J40" s="7">
+      <c r="J40" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="K40" s="9"/>
+      <c r="K40" s="7"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E41" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H41" s="7">
-        <v>1</v>
-      </c>
-      <c r="I41" s="7">
+      <c r="E41" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H41" s="5">
+        <v>1</v>
+      </c>
+      <c r="I41" s="5">
         <v>10</v>
       </c>
-      <c r="J41" s="7">
+      <c r="J41" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="K41" s="9"/>
+      <c r="K41" s="7"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="E42" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="F42" s="7" t="s">
+      <c r="F42" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G42" s="7" t="s">
+      <c r="G42" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="H42" s="7">
-        <v>1</v>
-      </c>
-      <c r="I42" s="7">
+      <c r="H42" s="5">
+        <v>1</v>
+      </c>
+      <c r="I42" s="5">
         <v>10</v>
       </c>
-      <c r="J42" s="7">
+      <c r="J42" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="K42" s="9" t="s">
+      <c r="K42" s="7" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E43" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G43" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H43" s="7">
-        <v>1</v>
-      </c>
-      <c r="I43" s="7">
+      <c r="E43" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H43" s="5">
+        <v>1</v>
+      </c>
+      <c r="I43" s="5">
         <v>10</v>
       </c>
-      <c r="J43" s="7">
+      <c r="J43" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="K43" s="9"/>
+      <c r="K43" s="7"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="E44" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="F44" s="7" t="s">
+      <c r="F44" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G44" s="12" t="s">
+      <c r="G44" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="H44" s="7">
-        <v>1</v>
-      </c>
-      <c r="I44" s="7">
+      <c r="H44" s="5">
+        <v>1</v>
+      </c>
+      <c r="I44" s="5">
         <v>50</v>
       </c>
-      <c r="J44" s="7">
+      <c r="J44" s="5">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="K44" s="9" t="s">
+      <c r="K44" s="7" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E45" s="7" t="s">
+      <c r="E45" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="F45" s="7" t="s">
+      <c r="F45" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G45" s="12" t="s">
+      <c r="G45" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="H45" s="7">
-        <v>1</v>
-      </c>
-      <c r="I45" s="7">
+      <c r="H45" s="5">
+        <v>1</v>
+      </c>
+      <c r="I45" s="5">
         <v>50</v>
       </c>
-      <c r="J45" s="7">
+      <c r="J45" s="5">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="K45" s="9"/>
+      <c r="K45" s="7"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E46" s="8" t="s">
+      <c r="E46" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="F46" s="8" t="s">
+      <c r="F46" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="G46" s="8" t="s">
+      <c r="G46" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="7">
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K46" s="9"/>
+      <c r="K46" s="16" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="E47" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="F47" s="8" t="s">
+      <c r="F47" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="G47" s="8" t="s">
+      <c r="G47" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="7">
+      <c r="H47" s="15"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K47" s="9"/>
+      <c r="K47" s="16" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="E48" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="F48" s="8" t="s">
+      <c r="F48" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="G48" s="8" t="s">
+      <c r="G48" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="H48" s="7"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="7">
+      <c r="H48" s="15"/>
+      <c r="I48" s="15"/>
+      <c r="J48" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K48" s="9"/>
+      <c r="K48" s="16" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C49" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="E49" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="F49" s="8" t="s">
+      <c r="F49" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="G49" s="8" t="s">
+      <c r="G49" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="H49" s="7"/>
-      <c r="I49" s="7"/>
-      <c r="J49" s="7">
+      <c r="H49" s="15"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K49" s="9"/>
+      <c r="K49" s="16" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A50" s="6"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7" t="s">
+      <c r="A50" s="4"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="F50" s="8"/>
-      <c r="G50" s="8" t="s">
+      <c r="F50" s="6"/>
+      <c r="G50" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="H50" s="7">
-        <v>1</v>
-      </c>
-      <c r="I50" s="7">
+      <c r="H50" s="5">
+        <v>1</v>
+      </c>
+      <c r="I50" s="5">
         <v>50</v>
       </c>
-      <c r="J50" s="7">
+      <c r="J50" s="5">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="K50" s="9"/>
+      <c r="K50" s="7"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A51" s="6"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7" t="s">
+      <c r="A51" s="4"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8" t="s">
+      <c r="F51" s="6"/>
+      <c r="G51" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="H51" s="7">
-        <v>1</v>
-      </c>
-      <c r="I51" s="7">
+      <c r="H51" s="5">
+        <v>1</v>
+      </c>
+      <c r="I51" s="5">
         <v>230</v>
       </c>
-      <c r="J51" s="7">
+      <c r="J51" s="5">
         <f t="shared" si="0"/>
         <v>230</v>
       </c>
-      <c r="K51" s="9"/>
+      <c r="K51" s="7"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A52" s="6"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7" t="s">
+      <c r="A52" s="4"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="F52" s="8"/>
-      <c r="G52" s="8" t="s">
+      <c r="F52" s="6"/>
+      <c r="G52" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="H52" s="7">
-        <v>1</v>
-      </c>
-      <c r="I52" s="7">
+      <c r="H52" s="5">
+        <v>1</v>
+      </c>
+      <c r="I52" s="5">
         <v>150</v>
       </c>
-      <c r="J52" s="7">
+      <c r="J52" s="5">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="K52" s="9"/>
+      <c r="K52" s="7"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A53" s="11" t="s">
+      <c r="A53" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C53" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="D53" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="E53" s="7" t="s">
+      <c r="E53" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="F53" s="7" t="s">
+      <c r="F53" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G53" s="7" t="s">
+      <c r="G53" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="H53" s="7">
-        <v>1</v>
-      </c>
-      <c r="I53" s="7">
+      <c r="H53" s="5">
+        <v>1</v>
+      </c>
+      <c r="I53" s="5">
         <v>4</v>
       </c>
-      <c r="J53" s="7">
+      <c r="J53" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="K53" s="9" t="s">
+      <c r="K53" s="7" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A54" s="6" t="s">
+      <c r="A54" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B54" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C54" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D54" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E54" s="7" t="s">
+      <c r="E54" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="F54" s="7" t="s">
+      <c r="F54" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G54" s="7" t="s">
+      <c r="G54" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="H54" s="7">
-        <v>1</v>
-      </c>
-      <c r="I54" s="7">
-        <v>1</v>
-      </c>
-      <c r="J54" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K54" s="9" t="s">
+      <c r="H54" s="5">
+        <v>1</v>
+      </c>
+      <c r="I54" s="5">
+        <v>1</v>
+      </c>
+      <c r="J54" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K54" s="7" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A55" s="6" t="s">
+      <c r="A55" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B55" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C55" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E55" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G55" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H55" s="7">
-        <v>1</v>
-      </c>
-      <c r="I55" s="7">
-        <v>1</v>
-      </c>
-      <c r="J55" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K55" s="9"/>
+      <c r="E55" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H55" s="5">
+        <v>1</v>
+      </c>
+      <c r="I55" s="5">
+        <v>1</v>
+      </c>
+      <c r="J55" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K55" s="7"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A56" s="6" t="s">
+      <c r="A56" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C56" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D56" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E56" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F56" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G56" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H56" s="7">
-        <v>1</v>
-      </c>
-      <c r="I56" s="7">
-        <v>1</v>
-      </c>
-      <c r="J56" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K56" s="9"/>
+      <c r="E56" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H56" s="5">
+        <v>1</v>
+      </c>
+      <c r="I56" s="5">
+        <v>1</v>
+      </c>
+      <c r="J56" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K56" s="7"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A57" s="6" t="s">
+      <c r="A57" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C57" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="D57" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E57" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G57" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H57" s="7">
-        <v>1</v>
-      </c>
-      <c r="I57" s="7">
-        <v>1</v>
-      </c>
-      <c r="J57" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K57" s="9"/>
+      <c r="E57" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H57" s="5">
+        <v>1</v>
+      </c>
+      <c r="I57" s="5">
+        <v>1</v>
+      </c>
+      <c r="J57" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K57" s="7"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A58" s="6" t="s">
+      <c r="A58" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B58" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C58" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="D58" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E58" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F58" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G58" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H58" s="7">
-        <v>1</v>
-      </c>
-      <c r="I58" s="7">
-        <v>1</v>
-      </c>
-      <c r="J58" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K58" s="9"/>
+      <c r="E58" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H58" s="5">
+        <v>1</v>
+      </c>
+      <c r="I58" s="5">
+        <v>1</v>
+      </c>
+      <c r="J58" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K58" s="7"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C59" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="D59" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E59" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F59" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G59" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H59" s="7">
-        <v>1</v>
-      </c>
-      <c r="I59" s="7">
-        <v>1</v>
-      </c>
-      <c r="J59" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K59" s="9"/>
+      <c r="E59" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H59" s="5">
+        <v>1</v>
+      </c>
+      <c r="I59" s="5">
+        <v>1</v>
+      </c>
+      <c r="J59" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K59" s="7"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A60" s="6" t="s">
+      <c r="A60" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B60" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C60" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="D60" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E60" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G60" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H60" s="7">
-        <v>1</v>
-      </c>
-      <c r="I60" s="7">
-        <v>1</v>
-      </c>
-      <c r="J60" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K60" s="9"/>
+      <c r="E60" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H60" s="5">
+        <v>1</v>
+      </c>
+      <c r="I60" s="5">
+        <v>1</v>
+      </c>
+      <c r="J60" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K60" s="7"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B61" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C61" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E61" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F61" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G61" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H61" s="7">
-        <v>1</v>
-      </c>
-      <c r="I61" s="7">
-        <v>1</v>
-      </c>
-      <c r="J61" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K61" s="9"/>
+      <c r="E61" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H61" s="5">
+        <v>1</v>
+      </c>
+      <c r="I61" s="5">
+        <v>1</v>
+      </c>
+      <c r="J61" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K61" s="7"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A62" s="6" t="s">
+      <c r="A62" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="B62" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C62" s="7" t="s">
+      <c r="C62" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D62" s="7" t="s">
+      <c r="D62" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E62" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F62" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G62" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H62" s="7">
-        <v>1</v>
-      </c>
-      <c r="I62" s="7">
-        <v>1</v>
-      </c>
-      <c r="J62" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K62" s="9"/>
+      <c r="E62" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H62" s="5">
+        <v>1</v>
+      </c>
+      <c r="I62" s="5">
+        <v>1</v>
+      </c>
+      <c r="J62" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K62" s="7"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A63" s="6" t="s">
+      <c r="A63" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B63" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="C63" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D63" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E63" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F63" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G63" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H63" s="7">
-        <v>1</v>
-      </c>
-      <c r="I63" s="7">
-        <v>1</v>
-      </c>
-      <c r="J63" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K63" s="9"/>
+      <c r="E63" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H63" s="5">
+        <v>1</v>
+      </c>
+      <c r="I63" s="5">
+        <v>1</v>
+      </c>
+      <c r="J63" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K63" s="7"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A64" s="6" t="s">
+      <c r="A64" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="B64" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C64" s="7" t="s">
+      <c r="C64" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D64" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E64" s="7" t="s">
+      <c r="E64" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="F64" s="7" t="s">
+      <c r="F64" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G64" s="7" t="s">
+      <c r="G64" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="H64" s="7">
-        <v>1</v>
-      </c>
-      <c r="I64" s="7">
-        <v>1</v>
-      </c>
-      <c r="J64" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K64" s="9" t="s">
+      <c r="H64" s="5">
+        <v>1</v>
+      </c>
+      <c r="I64" s="5">
+        <v>1</v>
+      </c>
+      <c r="J64" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K64" s="7" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A65" s="6" t="s">
+      <c r="A65" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B65" s="7" t="s">
+      <c r="B65" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="C65" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D65" s="7" t="s">
+      <c r="D65" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F65" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G65" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H65" s="7">
-        <v>1</v>
-      </c>
-      <c r="I65" s="7">
-        <v>1</v>
-      </c>
-      <c r="J65" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K65" s="9"/>
+      <c r="E65" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H65" s="5">
+        <v>1</v>
+      </c>
+      <c r="I65" s="5">
+        <v>1</v>
+      </c>
+      <c r="J65" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K65" s="7"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A66" s="6" t="s">
+      <c r="A66" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B66" s="7" t="s">
+      <c r="B66" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C66" s="7" t="s">
+      <c r="C66" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D66" s="7" t="s">
+      <c r="D66" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E66" s="7" t="s">
+      <c r="E66" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="F66" s="7" t="s">
+      <c r="F66" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G66" s="7" t="s">
+      <c r="G66" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="H66" s="7">
-        <v>1</v>
-      </c>
-      <c r="I66" s="7">
-        <v>1</v>
-      </c>
-      <c r="J66" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K66" s="9" t="s">
+      <c r="H66" s="5">
+        <v>1</v>
+      </c>
+      <c r="I66" s="5">
+        <v>1</v>
+      </c>
+      <c r="J66" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K66" s="7" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A67" s="6" t="s">
+      <c r="A67" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B67" s="7" t="s">
+      <c r="B67" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C67" s="7" t="s">
+      <c r="C67" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D67" s="7" t="s">
+      <c r="D67" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E67" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F67" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G67" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H67" s="7">
-        <v>1</v>
-      </c>
-      <c r="I67" s="7">
-        <v>1</v>
-      </c>
-      <c r="J67" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K67" s="9"/>
+      <c r="E67" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H67" s="5">
+        <v>1</v>
+      </c>
+      <c r="I67" s="5">
+        <v>1</v>
+      </c>
+      <c r="J67" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K67" s="7"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A68" s="6" t="s">
+      <c r="A68" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B68" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C68" s="7" t="s">
+      <c r="C68" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="D68" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E68" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F68" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G68" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H68" s="7">
-        <v>1</v>
-      </c>
-      <c r="I68" s="7">
-        <v>1</v>
-      </c>
-      <c r="J68" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K68" s="9"/>
+      <c r="E68" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H68" s="5">
+        <v>1</v>
+      </c>
+      <c r="I68" s="5">
+        <v>1</v>
+      </c>
+      <c r="J68" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K68" s="7"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A69" s="6" t="s">
+      <c r="A69" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B69" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="C69" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D69" s="7" t="s">
+      <c r="D69" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E69" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F69" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G69" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H69" s="7">
-        <v>1</v>
-      </c>
-      <c r="I69" s="7">
-        <v>1</v>
-      </c>
-      <c r="J69" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K69" s="9"/>
+      <c r="E69" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H69" s="5">
+        <v>1</v>
+      </c>
+      <c r="I69" s="5">
+        <v>1</v>
+      </c>
+      <c r="J69" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K69" s="7"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A70" s="13" t="s">
+      <c r="A70" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B70" s="14" t="s">
+      <c r="B70" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C70" s="14" t="s">
+      <c r="C70" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D70" s="14" t="s">
+      <c r="D70" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E70" s="16" t="s">
+      <c r="E70" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="F70" s="16" t="s">
+      <c r="F70" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="G70" s="16" t="s">
+      <c r="G70" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="H70" s="14"/>
-      <c r="I70" s="14"/>
-      <c r="J70" s="14">
+      <c r="H70" s="19"/>
+      <c r="I70" s="19"/>
+      <c r="J70" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K70" s="15" t="s">
+      <c r="K70" s="21" t="s">
         <v>194</v>
       </c>
     </row>
@@ -3935,15 +4056,15 @@
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="H73" s="14" t="s">
+      <c r="H73" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="I73" s="14"/>
-      <c r="J73" s="14">
+      <c r="I73" s="2"/>
+      <c r="J73" s="2">
         <f>J72*0.1</f>
         <v>488.20000000000005</v>
       </c>
-      <c r="K73" s="14" t="s">
+      <c r="K73" s="2" t="s">
         <v>223</v>
       </c>
     </row>
@@ -3989,10 +4110,10 @@
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="H78" s="14"/>
-      <c r="I78" s="14"/>
-      <c r="J78" s="14"/>
-      <c r="K78" s="14"/>
+      <c r="H78" s="2"/>
+      <c r="I78" s="2"/>
+      <c r="J78" s="2"/>
+      <c r="K78" s="2"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.4">
       <c r="H79" s="1" t="s">
@@ -4007,12 +4128,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A5:L79" xr:uid="{0250C408-8485-4A70-ADE7-CFBC4BEB7DFF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A54:T69">
     <sortCondition ref="B54:B69"/>
     <sortCondition ref="A54:A69"/>
   </sortState>
   <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" copies="0" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="51" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>